<commit_message>
view upload krs nilai
</commit_message>
<xml_diff>
--- a/backend/uploads/import_nilai/krs.xlsx
+++ b/backend/uploads/import_nilai/krs.xlsx
@@ -44,13 +44,13 @@
     <t>Kode Mata Kuliah</t>
   </si>
   <si>
-    <t>TM-11201-20</t>
+    <t>EE0103-19</t>
   </si>
   <si>
     <t>Nama Mata Kuliah</t>
   </si>
   <si>
-    <t>Agama</t>
+    <t>Matematika Diskret dan Logika</t>
   </si>
   <si>
     <t>Kelas</t>
@@ -62,10 +62,10 @@
     <t>Pengampu</t>
   </si>
   <si>
-    <t>Abdul Malik S.S., M.Hum</t>
-  </si>
-  <si>
-    <t>OITEmzrdecrvW/1vVNYUuA==</t>
+    <t>Dr.Ir. Augustinus Sujono M.T.</t>
+  </si>
+  <si>
+    <t>caFNPWvAHl//MJRM6J0jcw==</t>
   </si>
   <si>
     <t>No</t>
@@ -544,7 +544,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8">
-        <v>2019</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>